<commit_message>
Análisis limitaciones actividades básicas 28-11-21
</commit_message>
<xml_diff>
--- a/DATA/Pueblos.xlsx
+++ b/DATA/Pueblos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\INGENIERIA DE LA SALUD\3º UNI GIS\FUENTES DE DATOS BIOMEDICAS Y WEB SEMANTICAS\El precio de la discapacidad\El-precio-de-la-discapacidad\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB082B23-8C3D-48A1-AEE1-F1713CE7E7E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27A5776-C7C7-4235-90AE-FA10FB93309D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{3DD9CD08-5443-470D-A648-94C26439E4CC}"/>
   </bookViews>
@@ -60,9 +60,6 @@
     <t>Castilla y León</t>
   </si>
   <si>
-    <t>Castilla-La Mancha</t>
-  </si>
-  <si>
     <t>Cataluña</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>Número de municipios</t>
+  </si>
+  <si>
+    <t>Castilla - La Mancha</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
   <dimension ref="B3:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -554,7 +554,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -617,9 +617,9 @@
         <v>2248</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="3" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="C12" s="4">
         <v>919</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="13" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C13" s="2">
         <v>947</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="14" spans="2:3" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="2">
         <v>542</v>
@@ -643,7 +643,7 @@
     </row>
     <row r="15" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C15" s="2">
         <v>388</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="16" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C16" s="2">
         <v>313</v>
@@ -659,7 +659,7 @@
     </row>
     <row r="17" spans="2:3" ht="23.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" s="4">
         <v>179</v>
@@ -667,7 +667,7 @@
     </row>
     <row r="18" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C18" s="2">
         <v>45</v>
@@ -675,7 +675,7 @@
     </row>
     <row r="19" spans="2:3" ht="34.799999999999997" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="2">
         <v>272</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="20" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="2">
         <v>251</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="21" spans="2:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C21" s="2">
         <v>174</v>

</xml_diff>